<commit_message>
Updated tasks for Jan
</commit_message>
<xml_diff>
--- a/MonthlyStatusUpdate.xlsx
+++ b/MonthlyStatusUpdate.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="1" r:id="rId1"/>
     <sheet name="February" sheetId="2" r:id="rId2"/>
     <sheet name="March" sheetId="3" r:id="rId3"/>
+    <sheet name="April" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Nitesh</t>
   </si>
@@ -28,6 +29,18 @@
   </si>
   <si>
     <t>Pruthviraj</t>
+  </si>
+  <si>
+    <t>Migration Testing</t>
+  </si>
+  <si>
+    <t>Automation Testing</t>
+  </si>
+  <si>
+    <t>API Testing</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
   </si>
 </sst>
 </file>
@@ -359,16 +372,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:B6"/>
+  <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B3:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
@@ -391,20 +452,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -419,4 +466,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated names in Jan sheet
</commit_message>
<xml_diff>
--- a/MonthlyStatusUpdate.xlsx
+++ b/MonthlyStatusUpdate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,23 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Nitesh</t>
+  </si>
+  <si>
+    <t>Gautami</t>
+  </si>
+  <si>
+    <t>Pratiksha</t>
+  </si>
+  <si>
+    <t>Pruthviraj</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +359,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B3:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -370,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Updated tasks for Feb
</commit_message>
<xml_diff>
--- a/MonthlyStatusUpdate.xlsx
+++ b/MonthlyStatusUpdate.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Nitesh</t>
   </si>
@@ -375,7 +375,7 @@
   <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+      <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -423,32 +423,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:B6"/>
+  <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:2">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:2">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:2">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
       <c r="B6" t="s">
         <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>